<commit_message>
feat(admin): add Service Package Management
- Add PackagesManager component for BSI/BRI management\n- Integrate into Admin Dashboard\n- Add vehicle_type to service_packages schema\n- Update Configurator to filter by fuel type
</commit_message>
<xml_diff>
--- a/Kody modelowe x.xlsx
+++ b/Kody modelowe x.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="168">
   <si>
     <t>Table 1</t>
   </si>
@@ -176,6 +176,345 @@
   </si>
   <si>
     <t>520d xDrive Limuzyna</t>
+  </si>
+  <si>
+    <t>61CM</t>
+  </si>
+  <si>
+    <t>G42</t>
+  </si>
+  <si>
+    <t>Coupe</t>
+  </si>
+  <si>
+    <t>218i Coupe</t>
+  </si>
+  <si>
+    <t>RWD</t>
+  </si>
+  <si>
+    <t>11CN</t>
+  </si>
+  <si>
+    <t>220d Coupe</t>
+  </si>
+  <si>
+    <t>11CM</t>
+  </si>
+  <si>
+    <t>220i Coupe</t>
+  </si>
+  <si>
+    <t>21CM</t>
+  </si>
+  <si>
+    <t>230i Coupe</t>
+  </si>
+  <si>
+    <t>51FA</t>
+  </si>
+  <si>
+    <t>M240i xDrive Coupe</t>
+  </si>
+  <si>
+    <t>41GG</t>
+  </si>
+  <si>
+    <t>F74</t>
+  </si>
+  <si>
+    <t>216 Gran Coupe</t>
+  </si>
+  <si>
+    <t>11GH</t>
+  </si>
+  <si>
+    <t>218d Gran Coupe</t>
+  </si>
+  <si>
+    <t>31GH</t>
+  </si>
+  <si>
+    <t>220 Gran Coupe</t>
+  </si>
+  <si>
+    <t>21GH</t>
+  </si>
+  <si>
+    <t>220d Gran Coupe</t>
+  </si>
+  <si>
+    <t>71GG</t>
+  </si>
+  <si>
+    <t>223 xDrive Gran Coupe</t>
+  </si>
+  <si>
+    <t>31GG</t>
+  </si>
+  <si>
+    <t>M235 xDrive Gran Coupe</t>
+  </si>
+  <si>
+    <t>31DM</t>
+  </si>
+  <si>
+    <t>G87</t>
+  </si>
+  <si>
+    <t>Seria M</t>
+  </si>
+  <si>
+    <t>M2 CS Coupe</t>
+  </si>
+  <si>
+    <t>21DM</t>
+  </si>
+  <si>
+    <t>M2 Coupe</t>
+  </si>
+  <si>
+    <t>31HJ</t>
+  </si>
+  <si>
+    <t>G80</t>
+  </si>
+  <si>
+    <t>M3 Competition M xDrive Sedan</t>
+  </si>
+  <si>
+    <t>21HJ</t>
+  </si>
+  <si>
+    <t>M3 Competition Sedan</t>
+  </si>
+  <si>
+    <t>11HJ</t>
+  </si>
+  <si>
+    <t>M3 Sedan</t>
+  </si>
+  <si>
+    <t>31GB</t>
+  </si>
+  <si>
+    <t>G81</t>
+  </si>
+  <si>
+    <t>Touring</t>
+  </si>
+  <si>
+    <t>M3 CS Touring</t>
+  </si>
+  <si>
+    <t>21GB</t>
+  </si>
+  <si>
+    <t>28FU</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>Seria 3</t>
+  </si>
+  <si>
+    <t>318d Sedan</t>
+  </si>
+  <si>
+    <t>21FF</t>
+  </si>
+  <si>
+    <t>318i Sedan</t>
+  </si>
+  <si>
+    <t>28FF</t>
+  </si>
+  <si>
+    <t>38FU</t>
+  </si>
+  <si>
+    <t>320d Sedan</t>
+  </si>
+  <si>
+    <t>41FU</t>
+  </si>
+  <si>
+    <t>320d xDrive Sedan</t>
+  </si>
+  <si>
+    <t>48FU</t>
+  </si>
+  <si>
+    <t>58FF</t>
+  </si>
+  <si>
+    <t>320i Sedan</t>
+  </si>
+  <si>
+    <t>78FF</t>
+  </si>
+  <si>
+    <t>320i xDrive Sedan</t>
+  </si>
+  <si>
+    <t>71FF</t>
+  </si>
+  <si>
+    <t>58FU</t>
+  </si>
+  <si>
+    <t>330d xDrive Sedan</t>
+  </si>
+  <si>
+    <t>51FU</t>
+  </si>
+  <si>
+    <t>41GK</t>
+  </si>
+  <si>
+    <t>330e Sedan</t>
+  </si>
+  <si>
+    <t>48GK</t>
+  </si>
+  <si>
+    <t>51GK</t>
+  </si>
+  <si>
+    <t>330e xDrive Sedan</t>
+  </si>
+  <si>
+    <t>58GK</t>
+  </si>
+  <si>
+    <t>88FF</t>
+  </si>
+  <si>
+    <t>330i xDrive Sedan</t>
+  </si>
+  <si>
+    <t>81FF</t>
+  </si>
+  <si>
+    <t>68FU</t>
+  </si>
+  <si>
+    <t>M340d xDrive Sedan</t>
+  </si>
+  <si>
+    <t>61FU</t>
+  </si>
+  <si>
+    <t>61FT</t>
+  </si>
+  <si>
+    <t>M340i xDrive Sedan</t>
+  </si>
+  <si>
+    <t>68FT</t>
+  </si>
+  <si>
+    <t>11FZ</t>
+  </si>
+  <si>
+    <t>G21</t>
+  </si>
+  <si>
+    <t>318d Touring</t>
+  </si>
+  <si>
+    <t>11FY</t>
+  </si>
+  <si>
+    <t>318i Touring</t>
+  </si>
+  <si>
+    <t>21FZ</t>
+  </si>
+  <si>
+    <t>320d Touring</t>
+  </si>
+  <si>
+    <t>31FZ</t>
+  </si>
+  <si>
+    <t>320d xDrive Touring</t>
+  </si>
+  <si>
+    <t>21FY</t>
+  </si>
+  <si>
+    <t>320i Touring</t>
+  </si>
+  <si>
+    <t>51FZ</t>
+  </si>
+  <si>
+    <t>330d xDrive Touring</t>
+  </si>
+  <si>
+    <t>41GL</t>
+  </si>
+  <si>
+    <t>330e Touriung</t>
+  </si>
+  <si>
+    <t>51GL</t>
+  </si>
+  <si>
+    <t>330e xDrive Touring</t>
+  </si>
+  <si>
+    <t>71FY</t>
+  </si>
+  <si>
+    <t>330i xDrive Touring</t>
+  </si>
+  <si>
+    <t>61FZ</t>
+  </si>
+  <si>
+    <t>M340d xDrive Touring</t>
+  </si>
+  <si>
+    <t>21GL</t>
+  </si>
+  <si>
+    <t>M340i xDrive Touring</t>
+  </si>
+  <si>
+    <t>41BA</t>
+  </si>
+  <si>
+    <t>G83</t>
+  </si>
+  <si>
+    <t>Cabrio</t>
+  </si>
+  <si>
+    <t>M4 Competition M xDrive Cabrio</t>
+  </si>
+  <si>
+    <t>21HK</t>
+  </si>
+  <si>
+    <t>G82</t>
+  </si>
+  <si>
+    <t>M4 Competition Coupe</t>
+  </si>
+  <si>
+    <t>31HK</t>
+  </si>
+  <si>
+    <t>M4 Competition M xDrive Coupe</t>
+  </si>
+  <si>
+    <t>11HK</t>
+  </si>
+  <si>
+    <t>M4 Coupe</t>
   </si>
 </sst>
 </file>
@@ -342,7 +681,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -358,6 +697,9 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -368,7 +710,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -379,14 +727,29 @@
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1437,7 +1800,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:L23"/>
+  <dimension ref="A2:L77"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1445,7 +1808,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="12" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88281" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.0078" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.2734" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1406" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6562" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7656" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.22656" style="1" customWidth="1"/>
+    <col min="8" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.53125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.0781" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7266" style="1" customWidth="1"/>
     <col min="13" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1479,673 +1852,2617 @@
       <c r="E2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="4">
+      <c r="G2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="H2" t="s" s="4">
+      <c r="H2" t="s" s="5">
         <v>7</v>
       </c>
       <c r="I2" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="J2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="K2" t="s" s="4">
+      <c r="K2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="L2" t="s" s="4">
+      <c r="L2" t="s" s="5">
         <v>11</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" t="s" s="6">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" t="s" s="8">
         <v>14</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" t="s" s="8">
         <v>15</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>116</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="10">
         <v>122</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="10">
         <v>9.800000000000001</v>
       </c>
-      <c r="I3" t="s" s="7">
+      <c r="I3" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="J3" t="s" s="7">
+      <c r="J3" t="s" s="11">
         <v>17</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="10">
         <v>210</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="10">
         <v>380</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s" s="10">
+      <c r="A4" s="12"/>
+      <c r="B4" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="16">
         <v>150</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="16">
         <v>8.300000000000001</v>
       </c>
-      <c r="I4" t="s" s="11">
+      <c r="I4" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="J4" t="s" s="11">
+      <c r="J4" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="16">
         <v>222</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="16">
         <v>380</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" t="s" s="10">
+      <c r="A5" s="12"/>
+      <c r="B5" t="s" s="13">
         <v>21</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="18">
         <v>120</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="16">
         <v>170</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="16">
         <v>7.8</v>
       </c>
-      <c r="I5" t="s" s="11">
+      <c r="I5" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J5" t="s" s="11">
+      <c r="J5" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="16">
         <v>226</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="16">
         <v>300</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" t="s" s="10">
+      <c r="A6" s="12"/>
+      <c r="B6" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F6" t="s" s="11">
+      <c r="F6" t="s" s="15">
         <v>23</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="16">
         <v>163</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="16">
         <v>7.9</v>
       </c>
-      <c r="I6" t="s" s="11">
+      <c r="I6" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="J6" t="s" s="11">
+      <c r="J6" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="16">
         <v>222</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="16">
         <v>300</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" t="s" s="10">
+      <c r="A7" s="12"/>
+      <c r="B7" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F7" t="s" s="11">
+      <c r="F7" t="s" s="15">
         <v>25</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="16">
         <v>218</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="16">
         <v>6.3</v>
       </c>
-      <c r="I7" t="s" s="11">
+      <c r="I7" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J7" t="s" s="11">
+      <c r="J7" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="16">
         <v>246</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="16">
         <v>300</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" t="s" s="10">
+      <c r="A8" s="12"/>
+      <c r="B8" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="C8" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="D8" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E8" t="s" s="11">
+      <c r="E8" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F8" t="s" s="11">
+      <c r="F8" t="s" s="15">
         <v>28</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="16">
         <v>300</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="16">
         <v>4.9</v>
       </c>
-      <c r="I8" t="s" s="11">
+      <c r="I8" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J8" t="s" s="11">
+      <c r="J8" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="16">
         <v>250</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="16">
         <v>380</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" t="s" s="10">
+      <c r="A9" s="12"/>
+      <c r="B9" t="s" s="13">
         <v>29</v>
       </c>
-      <c r="C9" t="s" s="11">
+      <c r="C9" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D9" t="s" s="11">
+      <c r="D9" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E9" t="s" s="11">
+      <c r="E9" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F9" t="s" s="11">
+      <c r="F9" t="s" s="15">
         <v>32</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="16">
         <v>122</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="16">
         <v>10.3</v>
       </c>
-      <c r="I9" t="s" s="11">
+      <c r="I9" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J9" t="s" s="11">
+      <c r="J9" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="16">
         <v>206</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="16">
         <v>470</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" t="s" s="10">
+      <c r="A10" s="12"/>
+      <c r="B10" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="C10" t="s" s="11">
+      <c r="C10" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D10" t="s" s="11">
+      <c r="D10" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E10" t="s" s="11">
+      <c r="E10" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F10" t="s" s="11">
+      <c r="F10" t="s" s="15">
         <v>34</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="16">
         <v>150</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="16">
         <v>8.800000000000001</v>
       </c>
-      <c r="I10" t="s" s="11">
+      <c r="I10" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="J10" t="s" s="11">
+      <c r="J10" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="16">
         <v>220</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="16">
         <v>470</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" t="s" s="10">
+      <c r="A11" s="12"/>
+      <c r="B11" t="s" s="13">
         <v>35</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="C11" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D11" t="s" s="11">
+      <c r="D11" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E11" t="s" s="11">
+      <c r="E11" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F11" t="s" s="11">
+      <c r="F11" t="s" s="15">
         <v>36</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="16">
         <v>136</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="16">
         <v>9</v>
       </c>
-      <c r="I11" t="s" s="11">
+      <c r="I11" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J11" t="s" s="11">
+      <c r="J11" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="16">
         <v>214</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="16">
         <v>470</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" t="s" s="10">
+      <c r="A12" s="12"/>
+      <c r="B12" t="s" s="13">
         <v>37</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="C12" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D12" t="s" s="11">
+      <c r="D12" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E12" t="s" s="11">
+      <c r="E12" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F12" t="s" s="11">
+      <c r="F12" t="s" s="15">
         <v>38</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="16">
         <v>163</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="16">
         <v>8.300000000000001</v>
       </c>
-      <c r="I12" t="s" s="11">
+      <c r="I12" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="J12" t="s" s="11">
+      <c r="J12" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="16">
         <v>220</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="16">
         <v>415</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" t="s" s="10">
+      <c r="A13" s="12"/>
+      <c r="B13" t="s" s="13">
         <v>39</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D13" t="s" s="11">
+      <c r="D13" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E13" t="s" s="11">
+      <c r="E13" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F13" t="s" s="11">
+      <c r="F13" t="s" s="15">
         <v>40</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="16">
         <v>170</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="16">
         <v>8.1</v>
       </c>
-      <c r="I13" t="s" s="11">
+      <c r="I13" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J13" t="s" s="11">
+      <c r="J13" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="16">
         <v>221</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="16">
         <v>415</v>
       </c>
     </row>
-    <row r="14" ht="32.05" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" t="s" s="10">
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="12"/>
+      <c r="B14" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D14" t="s" s="11">
+      <c r="D14" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E14" t="s" s="11">
+      <c r="E14" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F14" t="s" s="11">
+      <c r="F14" t="s" s="15">
         <v>42</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="16">
         <v>211</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="16">
         <v>7.3</v>
       </c>
-      <c r="I14" t="s" s="11">
+      <c r="I14" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="J14" t="s" s="11">
+      <c r="J14" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="16">
         <v>233</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="16">
         <v>415</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" t="s" s="10">
+      <c r="A15" s="12"/>
+      <c r="B15" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D15" t="s" s="11">
+      <c r="D15" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E15" t="s" s="11">
+      <c r="E15" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F15" t="s" s="11">
+      <c r="F15" t="s" s="15">
         <v>44</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="16">
         <v>218</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="16">
         <v>6.9</v>
       </c>
-      <c r="I15" t="s" s="11">
+      <c r="I15" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="J15" t="s" s="11">
+      <c r="J15" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="16">
         <v>238</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="16">
         <v>415</v>
       </c>
     </row>
-    <row r="16" ht="32.05" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" t="s" s="10">
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="12"/>
+      <c r="B16" t="s" s="13">
         <v>45</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D16" t="s" s="11">
+      <c r="D16" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E16" t="s" s="11">
+      <c r="E16" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F16" t="s" s="11">
+      <c r="F16" t="s" s="15">
         <v>46</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="16">
         <v>245</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="16">
         <v>6.7</v>
       </c>
-      <c r="I16" t="s" s="11">
+      <c r="I16" t="s" s="14">
         <v>47</v>
       </c>
-      <c r="J16" t="s" s="11">
+      <c r="J16" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="16">
         <v>195</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="16">
         <v>406</v>
       </c>
     </row>
-    <row r="17" ht="32.05" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" t="s" s="10">
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" t="s" s="13">
         <v>48</v>
       </c>
-      <c r="C17" t="s" s="11">
+      <c r="C17" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="D17" t="s" s="11">
+      <c r="D17" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="E17" t="s" s="11">
+      <c r="E17" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F17" t="s" s="11">
+      <c r="F17" t="s" s="15">
         <v>49</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="16">
         <v>326</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="16">
         <v>5.5</v>
       </c>
-      <c r="I17" t="s" s="11">
+      <c r="I17" t="s" s="14">
         <v>47</v>
       </c>
-      <c r="J17" t="s" s="11">
+      <c r="J17" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="16">
         <v>205</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="16">
         <v>406</v>
       </c>
     </row>
-    <row r="18" ht="32.05" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" t="s" s="10">
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="12"/>
+      <c r="B18" t="s" s="13">
         <v>50</v>
       </c>
-      <c r="C18" t="s" s="11">
+      <c r="C18" t="s" s="14">
         <v>51</v>
       </c>
-      <c r="D18" t="s" s="11">
+      <c r="D18" t="s" s="14">
         <v>52</v>
       </c>
-      <c r="E18" t="s" s="11">
+      <c r="E18" t="s" s="14">
         <v>53</v>
       </c>
-      <c r="F18" t="s" s="11">
+      <c r="F18" t="s" s="15">
         <v>54</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="16">
         <v>197</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="16">
         <v>7.3</v>
       </c>
-      <c r="I18" t="s" s="11">
+      <c r="I18" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="J18" t="s" s="11">
+      <c r="J18" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="16">
         <v>228</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="16">
         <v>520</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" t="s" s="13">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s" s="15">
+        <v>58</v>
+      </c>
+      <c r="G19" s="16">
+        <v>156</v>
+      </c>
+      <c r="H19" s="16">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="I19" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K19" s="16">
+        <v>224</v>
+      </c>
+      <c r="L19" s="16">
+        <v>390</v>
+      </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s" s="15">
+        <v>61</v>
+      </c>
+      <c r="G20" s="16">
+        <v>190</v>
+      </c>
+      <c r="H20" s="16">
+        <v>6.9</v>
+      </c>
+      <c r="I20" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J20" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K20" s="16">
+        <v>237</v>
+      </c>
+      <c r="L20" s="16">
+        <v>390</v>
+      </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" t="s" s="13">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="G21" s="16">
+        <v>184</v>
+      </c>
+      <c r="H21" s="16">
+        <v>7.5</v>
+      </c>
+      <c r="I21" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K21" s="16">
+        <v>236</v>
+      </c>
+      <c r="L21" s="16">
+        <v>390</v>
+      </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" t="s" s="13">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s" s="15">
+        <v>65</v>
+      </c>
+      <c r="G22" s="16">
+        <v>245</v>
+      </c>
+      <c r="H22" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="I22" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K22" s="16">
+        <v>250</v>
+      </c>
+      <c r="L22" s="16">
+        <v>390</v>
+      </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
+      <c r="A23" s="12"/>
+      <c r="B23" t="s" s="13">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s" s="15">
+        <v>67</v>
+      </c>
+      <c r="G23" s="16">
+        <v>392</v>
+      </c>
+      <c r="H23" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="I23" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K23" s="16">
+        <v>250</v>
+      </c>
+      <c r="L23" s="16">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" s="12"/>
+      <c r="B24" t="s" s="13">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s" s="14">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s" s="15">
+        <v>70</v>
+      </c>
+      <c r="G24" s="16">
+        <v>122</v>
+      </c>
+      <c r="H24" s="16">
+        <v>9.9</v>
+      </c>
+      <c r="I24" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s" s="17">
+        <v>17</v>
+      </c>
+      <c r="K24" s="16">
+        <v>214</v>
+      </c>
+      <c r="L24" s="16">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" s="12"/>
+      <c r="B25" t="s" s="13">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s" s="14">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E25" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s" s="15">
+        <v>72</v>
+      </c>
+      <c r="G25" s="16">
+        <v>150</v>
+      </c>
+      <c r="H25" s="16">
+        <v>8.4</v>
+      </c>
+      <c r="I25" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J25" t="s" s="17">
+        <v>17</v>
+      </c>
+      <c r="K25" s="16">
+        <v>226</v>
+      </c>
+      <c r="L25" s="16">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" t="s" s="13">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s" s="14">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F26" t="s" s="15">
+        <v>74</v>
+      </c>
+      <c r="G26" s="16">
+        <v>170</v>
+      </c>
+      <c r="H26" s="16">
+        <v>7.9</v>
+      </c>
+      <c r="I26" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s" s="17">
+        <v>17</v>
+      </c>
+      <c r="K26" s="16">
+        <v>230</v>
+      </c>
+      <c r="L26" s="16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" s="12"/>
+      <c r="B27" t="s" s="13">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s" s="14">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s" s="15">
+        <v>76</v>
+      </c>
+      <c r="G27" s="16">
+        <v>163</v>
+      </c>
+      <c r="H27" s="16">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J27" t="s" s="17">
+        <v>17</v>
+      </c>
+      <c r="K27" s="16">
+        <v>226</v>
+      </c>
+      <c r="L27" s="16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" t="s" s="13">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s" s="14">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="G28" s="16">
+        <v>218</v>
+      </c>
+      <c r="H28" s="16">
+        <v>6.4</v>
+      </c>
+      <c r="I28" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J28" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K28" s="16">
+        <v>250</v>
+      </c>
+      <c r="L28" s="16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" s="12"/>
+      <c r="B29" t="s" s="13">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s" s="14">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F29" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="G29" s="16">
+        <v>300</v>
+      </c>
+      <c r="H29" s="16">
+        <v>4.9</v>
+      </c>
+      <c r="I29" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J29" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K29" s="16">
+        <v>250</v>
+      </c>
+      <c r="L29" s="16">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" t="s" s="13">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s" s="14">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F30" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="G30" s="16">
+        <v>530</v>
+      </c>
+      <c r="H30" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="I30" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J30" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K30" s="16">
+        <v>302</v>
+      </c>
+      <c r="L30" s="16">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" s="12"/>
+      <c r="B31" t="s" s="13">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s" s="14">
+        <v>82</v>
+      </c>
+      <c r="D31" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F31" t="s" s="15">
+        <v>86</v>
+      </c>
+      <c r="G31" s="16">
+        <v>480</v>
+      </c>
+      <c r="H31" s="16">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J31" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K31" s="16">
+        <v>250</v>
+      </c>
+      <c r="L31" s="16">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" s="12"/>
+      <c r="B32" t="s" s="13">
+        <v>87</v>
+      </c>
+      <c r="C32" t="s" s="14">
+        <v>88</v>
+      </c>
+      <c r="D32" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E32" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="G32" s="16">
+        <v>530</v>
+      </c>
+      <c r="H32" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="I32" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J32" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K32" s="16">
+        <v>250</v>
+      </c>
+      <c r="L32" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" s="12"/>
+      <c r="B33" t="s" s="13">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s" s="14">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F33" t="s" s="15">
+        <v>91</v>
+      </c>
+      <c r="G33" s="16">
+        <v>510</v>
+      </c>
+      <c r="H33" s="16">
+        <v>3.9</v>
+      </c>
+      <c r="I33" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J33" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K33" s="16">
+        <v>250</v>
+      </c>
+      <c r="L33" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" s="12"/>
+      <c r="B34" t="s" s="13">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s" s="14">
+        <v>88</v>
+      </c>
+      <c r="D34" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E34" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s" s="15">
+        <v>93</v>
+      </c>
+      <c r="G34" s="16">
+        <v>480</v>
+      </c>
+      <c r="H34" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="I34" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J34" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K34" s="16">
+        <v>250</v>
+      </c>
+      <c r="L34" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" s="12"/>
+      <c r="B35" t="s" s="13">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s" s="14">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F35" t="s" s="15">
+        <v>97</v>
+      </c>
+      <c r="G35" s="16">
+        <v>551</v>
+      </c>
+      <c r="H35" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="I35" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J35" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K35" s="16">
+        <v>300</v>
+      </c>
+      <c r="L35" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" s="12"/>
+      <c r="B36" t="s" s="13">
+        <v>98</v>
+      </c>
+      <c r="C36" t="s" s="14">
+        <v>95</v>
+      </c>
+      <c r="D36" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F36" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="G36" s="16">
+        <v>530</v>
+      </c>
+      <c r="H36" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="I36" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J36" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K36" s="16">
+        <v>250</v>
+      </c>
+      <c r="L36" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" s="12"/>
+      <c r="B37" t="s" s="13">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E37" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F37" t="s" s="15">
+        <v>102</v>
+      </c>
+      <c r="G37" s="16">
+        <v>150</v>
+      </c>
+      <c r="H37" s="16">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="I37" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J37" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K37" s="16">
+        <v>218</v>
+      </c>
+      <c r="L37" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" s="12"/>
+      <c r="B38" t="s" s="13">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D38" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E38" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F38" t="s" s="15">
+        <v>104</v>
+      </c>
+      <c r="G38" s="16">
+        <v>156</v>
+      </c>
+      <c r="H38" s="16">
+        <v>8.6</v>
+      </c>
+      <c r="I38" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J38" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K38" s="16">
+        <v>223</v>
+      </c>
+      <c r="L38" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" s="12"/>
+      <c r="B39" t="s" s="13">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D39" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E39" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F39" t="s" s="15">
+        <v>104</v>
+      </c>
+      <c r="G39" s="16">
+        <v>156</v>
+      </c>
+      <c r="H39" s="16">
+        <v>8.6</v>
+      </c>
+      <c r="I39" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J39" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K39" s="16">
+        <v>223</v>
+      </c>
+      <c r="L39" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" s="12"/>
+      <c r="B40" t="s" s="13">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E40" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s" s="15">
+        <v>107</v>
+      </c>
+      <c r="G40" s="16">
+        <v>190</v>
+      </c>
+      <c r="H40" s="16">
+        <v>6.9</v>
+      </c>
+      <c r="I40" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J40" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K40" s="16">
+        <v>235</v>
+      </c>
+      <c r="L40" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" s="12"/>
+      <c r="B41" t="s" s="13">
+        <v>108</v>
+      </c>
+      <c r="C41" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E41" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F41" t="s" s="15">
+        <v>109</v>
+      </c>
+      <c r="G41" s="16">
+        <v>190</v>
+      </c>
+      <c r="H41" s="16">
+        <v>7.2</v>
+      </c>
+      <c r="I41" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J41" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K41" s="16">
+        <v>228</v>
+      </c>
+      <c r="L41" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" s="12"/>
+      <c r="B42" t="s" s="13">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D42" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E42" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F42" t="s" s="15">
+        <v>109</v>
+      </c>
+      <c r="G42" s="16">
+        <v>190</v>
+      </c>
+      <c r="H42" s="16">
+        <v>7.2</v>
+      </c>
+      <c r="I42" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J42" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K42" s="16">
+        <v>228</v>
+      </c>
+      <c r="L42" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" s="12"/>
+      <c r="B43" t="s" s="13">
+        <v>111</v>
+      </c>
+      <c r="C43" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E43" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F43" t="s" s="15">
+        <v>112</v>
+      </c>
+      <c r="G43" s="16">
+        <v>184</v>
+      </c>
+      <c r="H43" s="16">
+        <v>7.4</v>
+      </c>
+      <c r="I43" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J43" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K43" s="16">
+        <v>235</v>
+      </c>
+      <c r="L43" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" s="12"/>
+      <c r="B44" t="s" s="13">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D44" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E44" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F44" t="s" s="15">
+        <v>114</v>
+      </c>
+      <c r="G44" s="16">
+        <v>184</v>
+      </c>
+      <c r="H44" s="16">
+        <v>7.7</v>
+      </c>
+      <c r="I44" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J44" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K44" s="16">
+        <v>230</v>
+      </c>
+      <c r="L44" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="45" ht="20.05" customHeight="1">
+      <c r="A45" s="12"/>
+      <c r="B45" t="s" s="13">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D45" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E45" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F45" t="s" s="15">
+        <v>114</v>
+      </c>
+      <c r="G45" s="16">
+        <v>184</v>
+      </c>
+      <c r="H45" s="16">
+        <v>7.7</v>
+      </c>
+      <c r="I45" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J45" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K45" s="16">
+        <v>230</v>
+      </c>
+      <c r="L45" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="46" ht="20.05" customHeight="1">
+      <c r="A46" s="12"/>
+      <c r="B46" t="s" s="13">
+        <v>116</v>
+      </c>
+      <c r="C46" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D46" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E46" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F46" t="s" s="15">
+        <v>117</v>
+      </c>
+      <c r="G46" s="16">
+        <v>286</v>
+      </c>
+      <c r="H46" s="16">
+        <v>5</v>
+      </c>
+      <c r="I46" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J46" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K46" s="16">
+        <v>250</v>
+      </c>
+      <c r="L46" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="47" ht="20.05" customHeight="1">
+      <c r="A47" s="12"/>
+      <c r="B47" t="s" s="13">
+        <v>118</v>
+      </c>
+      <c r="C47" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E47" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F47" t="s" s="15">
+        <v>117</v>
+      </c>
+      <c r="G47" s="16">
+        <v>286</v>
+      </c>
+      <c r="H47" s="16">
+        <v>5</v>
+      </c>
+      <c r="I47" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K47" s="16">
+        <v>250</v>
+      </c>
+      <c r="L47" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="48" ht="20.05" customHeight="1">
+      <c r="A48" s="12"/>
+      <c r="B48" t="s" s="13">
+        <v>119</v>
+      </c>
+      <c r="C48" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E48" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F48" t="s" s="15">
+        <v>120</v>
+      </c>
+      <c r="G48" s="16">
+        <v>292</v>
+      </c>
+      <c r="H48" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="I48" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="J48" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K48" s="16">
+        <v>230</v>
+      </c>
+      <c r="L48" s="16">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="49" ht="20.05" customHeight="1">
+      <c r="A49" s="12"/>
+      <c r="B49" t="s" s="13">
+        <v>121</v>
+      </c>
+      <c r="C49" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E49" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F49" t="s" s="15">
+        <v>120</v>
+      </c>
+      <c r="G49" s="16">
+        <v>292</v>
+      </c>
+      <c r="H49" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="I49" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="J49" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K49" s="16">
+        <v>230</v>
+      </c>
+      <c r="L49" s="16">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="50" ht="20.05" customHeight="1">
+      <c r="A50" s="12"/>
+      <c r="B50" t="s" s="13">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D50" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E50" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F50" t="s" s="15">
+        <v>123</v>
+      </c>
+      <c r="G50" s="16">
+        <v>292</v>
+      </c>
+      <c r="H50" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="I50" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="J50" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K50" s="16">
+        <v>230</v>
+      </c>
+      <c r="L50" s="16">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" ht="20.05" customHeight="1">
+      <c r="A51" s="12"/>
+      <c r="B51" t="s" s="13">
+        <v>124</v>
+      </c>
+      <c r="C51" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E51" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F51" t="s" s="15">
+        <v>123</v>
+      </c>
+      <c r="G51" s="16">
+        <v>292</v>
+      </c>
+      <c r="H51" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="I51" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="J51" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K51" s="16">
+        <v>230</v>
+      </c>
+      <c r="L51" s="16">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="52" ht="20.05" customHeight="1">
+      <c r="A52" s="12"/>
+      <c r="B52" t="s" s="13">
+        <v>125</v>
+      </c>
+      <c r="C52" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E52" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F52" t="s" s="15">
+        <v>126</v>
+      </c>
+      <c r="G52" s="16">
+        <v>245</v>
+      </c>
+      <c r="H52" s="16">
+        <v>5.7</v>
+      </c>
+      <c r="I52" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J52" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K52" s="16">
+        <v>250</v>
+      </c>
+      <c r="L52" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="53" ht="20.05" customHeight="1">
+      <c r="A53" s="12"/>
+      <c r="B53" t="s" s="13">
+        <v>127</v>
+      </c>
+      <c r="C53" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D53" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E53" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s" s="15">
+        <v>126</v>
+      </c>
+      <c r="G53" s="16">
+        <v>245</v>
+      </c>
+      <c r="H53" s="16">
+        <v>5.7</v>
+      </c>
+      <c r="I53" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J53" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K53" s="16">
+        <v>250</v>
+      </c>
+      <c r="L53" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" s="12"/>
+      <c r="B54" t="s" s="13">
+        <v>128</v>
+      </c>
+      <c r="C54" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D54" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E54" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s" s="15">
+        <v>129</v>
+      </c>
+      <c r="G54" s="16">
+        <v>340</v>
+      </c>
+      <c r="H54" s="16">
+        <v>4.6</v>
+      </c>
+      <c r="I54" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J54" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K54" s="16">
+        <v>250</v>
+      </c>
+      <c r="L54" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" s="12"/>
+      <c r="B55" t="s" s="13">
+        <v>130</v>
+      </c>
+      <c r="C55" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D55" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E55" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s" s="15">
+        <v>129</v>
+      </c>
+      <c r="G55" s="16">
+        <v>340</v>
+      </c>
+      <c r="H55" s="16">
+        <v>4.6</v>
+      </c>
+      <c r="I55" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J55" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K55" s="16">
+        <v>250</v>
+      </c>
+      <c r="L55" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="56" ht="20.05" customHeight="1">
+      <c r="A56" s="12"/>
+      <c r="B56" t="s" s="13">
+        <v>131</v>
+      </c>
+      <c r="C56" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D56" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E56" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F56" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="G56" s="16">
+        <v>392</v>
+      </c>
+      <c r="H56" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="I56" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J56" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K56" s="16">
+        <v>250</v>
+      </c>
+      <c r="L56" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="57" ht="20.05" customHeight="1">
+      <c r="A57" s="12"/>
+      <c r="B57" t="s" s="13">
+        <v>133</v>
+      </c>
+      <c r="C57" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="D57" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E57" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="F57" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="G57" s="16">
+        <v>392</v>
+      </c>
+      <c r="H57" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="I57" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J57" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K57" s="16">
+        <v>250</v>
+      </c>
+      <c r="L57" s="16">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="58" ht="20.05" customHeight="1">
+      <c r="A58" s="12"/>
+      <c r="B58" t="s" s="13">
+        <v>134</v>
+      </c>
+      <c r="C58" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D58" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E58" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F58" t="s" s="15">
+        <v>136</v>
+      </c>
+      <c r="G58" s="16">
+        <v>150</v>
+      </c>
+      <c r="H58" s="16">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="I58" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J58" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K58" s="16">
+        <v>213</v>
+      </c>
+      <c r="L58" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" ht="20.05" customHeight="1">
+      <c r="A59" s="12"/>
+      <c r="B59" t="s" s="13">
+        <v>137</v>
+      </c>
+      <c r="C59" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D59" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E59" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F59" t="s" s="15">
+        <v>138</v>
+      </c>
+      <c r="G59" s="16">
+        <v>156</v>
+      </c>
+      <c r="H59" s="16">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="I59" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J59" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K59" s="16">
+        <v>218</v>
+      </c>
+      <c r="L59" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" ht="20.05" customHeight="1">
+      <c r="A60" s="12"/>
+      <c r="B60" t="s" s="13">
+        <v>139</v>
+      </c>
+      <c r="C60" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D60" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E60" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F60" t="s" s="15">
+        <v>140</v>
+      </c>
+      <c r="G60" s="16">
+        <v>190</v>
+      </c>
+      <c r="H60" s="16">
+        <v>7.2</v>
+      </c>
+      <c r="I60" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J60" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K60" s="16">
+        <v>229</v>
+      </c>
+      <c r="L60" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" ht="20.05" customHeight="1">
+      <c r="A61" s="12"/>
+      <c r="B61" t="s" s="13">
+        <v>141</v>
+      </c>
+      <c r="C61" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D61" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E61" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F61" t="s" s="15">
+        <v>142</v>
+      </c>
+      <c r="G61" s="16">
+        <v>190</v>
+      </c>
+      <c r="H61" s="16">
+        <v>7.5</v>
+      </c>
+      <c r="I61" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J61" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K61" s="16">
+        <v>225</v>
+      </c>
+      <c r="L61" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" ht="20.05" customHeight="1">
+      <c r="A62" s="12"/>
+      <c r="B62" t="s" s="13">
+        <v>143</v>
+      </c>
+      <c r="C62" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D62" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E62" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F62" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="G62" s="16">
+        <v>184</v>
+      </c>
+      <c r="H62" s="16">
+        <v>7.6</v>
+      </c>
+      <c r="I62" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J62" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K62" s="16">
+        <v>230</v>
+      </c>
+      <c r="L62" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" ht="20.05" customHeight="1">
+      <c r="A63" s="12"/>
+      <c r="B63" t="s" s="13">
+        <v>145</v>
+      </c>
+      <c r="C63" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D63" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E63" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F63" t="s" s="15">
+        <v>146</v>
+      </c>
+      <c r="G63" s="16">
+        <v>286</v>
+      </c>
+      <c r="H63" s="16">
+        <v>5.2</v>
+      </c>
+      <c r="I63" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J63" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K63" s="16">
+        <v>250</v>
+      </c>
+      <c r="L63" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" ht="20.05" customHeight="1">
+      <c r="A64" s="12"/>
+      <c r="B64" t="s" s="13">
+        <v>147</v>
+      </c>
+      <c r="C64" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D64" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E64" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F64" t="s" s="15">
+        <v>148</v>
+      </c>
+      <c r="G64" s="16">
+        <v>292</v>
+      </c>
+      <c r="H64" s="16">
+        <v>6</v>
+      </c>
+      <c r="I64" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="J64" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K64" s="16">
+        <v>230</v>
+      </c>
+      <c r="L64" s="16">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="65" ht="20.05" customHeight="1">
+      <c r="A65" s="12"/>
+      <c r="B65" t="s" s="13">
+        <v>149</v>
+      </c>
+      <c r="C65" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D65" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E65" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F65" t="s" s="15">
+        <v>150</v>
+      </c>
+      <c r="G65" s="16">
+        <v>292</v>
+      </c>
+      <c r="H65" s="16">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="J65" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K65" s="16">
+        <v>230</v>
+      </c>
+      <c r="L65" s="16">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="66" ht="20.05" customHeight="1">
+      <c r="A66" s="12"/>
+      <c r="B66" t="s" s="13">
+        <v>151</v>
+      </c>
+      <c r="C66" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D66" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E66" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F66" t="s" s="15">
+        <v>152</v>
+      </c>
+      <c r="G66" s="16">
+        <v>245</v>
+      </c>
+      <c r="H66" s="16">
+        <v>6</v>
+      </c>
+      <c r="I66" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J66" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K66" s="16">
+        <v>250</v>
+      </c>
+      <c r="L66" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" ht="20.05" customHeight="1">
+      <c r="A67" s="12"/>
+      <c r="B67" t="s" s="13">
+        <v>153</v>
+      </c>
+      <c r="C67" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D67" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E67" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F67" t="s" s="15">
+        <v>154</v>
+      </c>
+      <c r="G67" s="16">
+        <v>340</v>
+      </c>
+      <c r="H67" s="16">
+        <v>4.7</v>
+      </c>
+      <c r="I67" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="J67" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K67" s="16">
+        <v>250</v>
+      </c>
+      <c r="L67" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="68" ht="20.05" customHeight="1">
+      <c r="A68" s="12"/>
+      <c r="B68" t="s" s="13">
+        <v>155</v>
+      </c>
+      <c r="C68" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="D68" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="E68" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F68" t="s" s="15">
+        <v>156</v>
+      </c>
+      <c r="G68" s="16">
+        <v>392</v>
+      </c>
+      <c r="H68" s="16">
+        <v>4.5</v>
+      </c>
+      <c r="I68" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J68" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K68" s="16">
+        <v>250</v>
+      </c>
+      <c r="L68" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="69" ht="20.05" customHeight="1">
+      <c r="A69" s="12"/>
+      <c r="B69" t="s" s="13">
+        <v>157</v>
+      </c>
+      <c r="C69" t="s" s="14">
+        <v>158</v>
+      </c>
+      <c r="D69" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E69" t="s" s="14">
+        <v>159</v>
+      </c>
+      <c r="F69" t="s" s="15">
+        <v>160</v>
+      </c>
+      <c r="G69" s="16">
+        <v>530</v>
+      </c>
+      <c r="H69" s="16">
+        <v>3.7</v>
+      </c>
+      <c r="I69" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J69" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K69" s="16">
+        <v>250</v>
+      </c>
+      <c r="L69" s="16">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="70" ht="20.05" customHeight="1">
+      <c r="A70" s="12"/>
+      <c r="B70" t="s" s="13">
+        <v>161</v>
+      </c>
+      <c r="C70" t="s" s="14">
+        <v>162</v>
+      </c>
+      <c r="D70" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E70" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F70" t="s" s="15">
+        <v>163</v>
+      </c>
+      <c r="G70" s="16">
+        <v>510</v>
+      </c>
+      <c r="H70" s="16">
+        <v>3.9</v>
+      </c>
+      <c r="I70" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J70" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K70" s="16">
+        <v>250</v>
+      </c>
+      <c r="L70" s="16">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="71" ht="20.05" customHeight="1">
+      <c r="A71" s="12"/>
+      <c r="B71" t="s" s="13">
+        <v>164</v>
+      </c>
+      <c r="C71" t="s" s="14">
+        <v>162</v>
+      </c>
+      <c r="D71" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E71" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F71" t="s" s="15">
+        <v>165</v>
+      </c>
+      <c r="G71" s="16">
+        <v>530</v>
+      </c>
+      <c r="H71" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="I71" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J71" t="s" s="17">
+        <v>26</v>
+      </c>
+      <c r="K71" s="16">
+        <v>250</v>
+      </c>
+      <c r="L71" s="16">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="72" ht="20.05" customHeight="1">
+      <c r="A72" s="12"/>
+      <c r="B72" t="s" s="13">
+        <v>166</v>
+      </c>
+      <c r="C72" t="s" s="14">
+        <v>162</v>
+      </c>
+      <c r="D72" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="E72" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="F72" t="s" s="15">
+        <v>167</v>
+      </c>
+      <c r="G72" s="16">
+        <v>480</v>
+      </c>
+      <c r="H72" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="I72" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="J72" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="K72" s="16">
+        <v>250</v>
+      </c>
+      <c r="L72" s="16">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="73" ht="20.05" customHeight="1">
+      <c r="A73" s="12"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="22"/>
+    </row>
+    <row r="74" ht="20.05" customHeight="1">
+      <c r="A74" s="12"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="22"/>
+      <c r="L74" s="22"/>
+    </row>
+    <row r="75" ht="20.05" customHeight="1">
+      <c r="A75" s="12"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="20"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="22"/>
+      <c r="L75" s="22"/>
+    </row>
+    <row r="76" ht="20.05" customHeight="1">
+      <c r="A76" s="12"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="22"/>
+      <c r="L76" s="22"/>
+    </row>
+    <row r="77" ht="20.05" customHeight="1">
+      <c r="A77" s="12"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="22"/>
+      <c r="L77" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>